<commit_message>
D: fixed supporting openoffice by translation files. fixed tests. KP-7471
</commit_message>
<xml_diff>
--- a/src/Tests/WB.Tests.Unit.Designer/BoundedContexts/Designer/TranslationServiceTests/testTranslations.xlsx
+++ b/src/Tests/WB.Tests.Unit.Designer/BoundedContexts/Designer/TranslationServiceTests/testTranslations.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\surveysolutions\src\Tests\WB.Tests.Unit.Designer\BoundedContexts\Designer\TranslationServiceTests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\surveysolutions\src\Tests\WB.Tests.Unit.Designer\BoundedContexts\Designer\TranslationServiceTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13800"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Translations" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Type</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Index</t>
   </si>
   <si>
-    <t>Id</t>
-  </si>
-  <si>
     <t>Original</t>
   </si>
   <si>
@@ -57,6 +54,21 @@
   </si>
   <si>
     <t>option</t>
+  </si>
+  <si>
+    <t>Entity Id</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>ValidationMessage</t>
+  </si>
+  <si>
+    <t>Instruction</t>
+  </si>
+  <si>
+    <t>OptionTitle</t>
   </si>
 </sst>
 </file>
@@ -96,7 +108,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -112,9 +124,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Офіс">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -152,7 +164,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Офіс">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -258,7 +270,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Офіс">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -411,92 +423,94 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="54.28515625" customWidth="1"/>
+    <col min="1" max="1" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Designer: added test for import excel with multiple sheets. KP-7552
</commit_message>
<xml_diff>
--- a/src/Tests/WB.Tests.Unit.Designer/BoundedContexts/Designer/TranslationServiceTests/testTranslations.xlsx
+++ b/src/Tests/WB.Tests.Unit.Designer/BoundedContexts/Designer/TranslationServiceTests/testTranslations.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\surveysolutions\src\Tests\WB.Tests.Unit.Designer\BoundedContexts\Designer\TranslationServiceTests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SurveySolutions\src\Tests\WB.Tests.Unit.Designer\BoundedContexts\Designer\TranslationServiceTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Translations" sheetId="1" r:id="rId1"/>
+    <sheet name="Translations question" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>Type</t>
   </si>
@@ -69,6 +70,15 @@
   </si>
   <si>
     <t>OptionTitle</t>
+  </si>
+  <si>
+    <t>Combobox Option</t>
+  </si>
+  <si>
+    <t>Опция Комбобокса</t>
+  </si>
+  <si>
+    <t>11111111111111111111111111111111</t>
   </si>
 </sst>
 </file>
@@ -104,11 +114,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -124,9 +135,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Офіс">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -164,7 +175,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Офіс">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -270,7 +281,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Офіс">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -422,9 +433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -517,4 +526,61 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
D: generating worksheet name for filtered/cascading questions. added tests KP-7577
</commit_message>
<xml_diff>
--- a/src/Tests/WB.Tests.Unit.Designer/BoundedContexts/Designer/TranslationServiceTests/testTranslations.xlsx
+++ b/src/Tests/WB.Tests.Unit.Designer/BoundedContexts/Designer/TranslationServiceTests/testTranslations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SurveySolutions\src\Tests\WB.Tests.Unit.Designer\BoundedContexts\Designer\TranslationServiceTests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\surveysolutions\src\Tests\WB.Tests.Unit.Designer\BoundedContexts\Designer\TranslationServiceTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Translations" sheetId="1" r:id="rId1"/>
-    <sheet name="Translations question" sheetId="2" r:id="rId2"/>
+    <sheet name="@@_question" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -119,7 +119,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -135,9 +135,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Офіс">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -175,7 +175,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Офіс">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -281,7 +281,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Офіс">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>

</xml_diff>

<commit_message>
KP-11725 D: Extension of questionnaire's translation files
</commit_message>
<xml_diff>
--- a/src/Tests/WB.Tests.Unit.Designer/BoundedContexts/Designer/TranslationServiceTests/testTranslations.xlsx
+++ b/src/Tests/WB.Tests.Unit.Designer/BoundedContexts/Designer/TranslationServiceTests/testTranslations.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\surveysolutions\src\Tests\WB.Tests.Unit.Designer\BoundedContexts\Designer\TranslationServiceTests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\surveysolutions\src\Tests\WB.Tests.Unit.Designer\BoundedContexts\Designer\TranslationServiceTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13800" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13800"/>
   </bookViews>
   <sheets>
     <sheet name="Translations" sheetId="1" r:id="rId1"/>
     <sheet name="@@_question" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>Type</t>
   </si>
@@ -79,12 +79,18 @@
   </si>
   <si>
     <t>11111111111111111111111111111111</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>c1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,7 +125,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -431,94 +437,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.85546875" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -530,52 +554,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>